<commit_message>
Added indent and subheader configuration to the scafolder; Added support for unpublished module items; Added config for frontend frameworks
</commit_message>
<xml_diff>
--- a/folder_template/config.xlsx
+++ b/folder_template/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joren\Documents\repositories\CanvasCourseScaffolder\folder_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\canvas-course-scaffolder-with-course-configs\folder_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BD74EB-D8CA-4C19-8319-0491DC51BF13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B8D9047-6C78-40AF-81D7-119259C59FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Algemene info" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="75">
   <si>
     <t>Naam</t>
   </si>
@@ -268,6 +268,9 @@
   </si>
   <si>
     <t>Toets (indien toets)</t>
+  </si>
+  <si>
+    <t>Indentatie niveau (leeg laten of 0 invullen indien indentatie niet nodig is)</t>
   </si>
 </sst>
 </file>
@@ -325,7 +328,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,9 +418,9 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}" name="Tabel3567" displayName="Tabel3567" ref="A1:H13" totalsRowShown="0">
-  <autoFilter ref="A1:H13" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}" name="Tabel3567" displayName="Tabel3567" ref="A1:I13" totalsRowShown="0">
+  <autoFilter ref="A1:I13" xr:uid="{B8351439-171F-43CA-8A27-46439B0C8D5A}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4F1B940E-7EAD-48A5-AA1E-A5E5ED525C5C}" name="Module"/>
     <tableColumn id="2" xr3:uid="{54A84E46-41BB-4012-84B6-2A4A1FB473F4}" name="Type"/>
     <tableColumn id="7" xr3:uid="{0D1BF778-48C7-4B21-B7BE-8990087F8BB9}" name="Weergavenaam"/>
@@ -426,6 +429,7 @@
     <tableColumn id="9" xr3:uid="{AB31A007-9997-44CA-85E7-F51F89C6EA51}" name="Link (indien externe url)"/>
     <tableColumn id="12" xr3:uid="{A4C6EB42-0E3A-461A-A526-712FC10E2F84}" name="Toets (indien toets)"/>
     <tableColumn id="3" xr3:uid="{6BB9FB76-0628-413E-8494-657C4EE45BC1}" name="Naam van bestand (indien bestand)"/>
+    <tableColumn id="4" xr3:uid="{125D0D81-9039-4750-89E3-C075946A08B3}" name="Indentatie niveau (leeg laten of 0 invullen indien indentatie niet nodig is)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -708,15 +712,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="123.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -724,7 +728,7 @@
         <v>10139</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -732,7 +736,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -740,7 +744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -748,7 +752,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -776,13 +780,13 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -790,7 +794,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -798,7 +802,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -806,7 +810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -830,19 +834,19 @@
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -868,7 +872,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -886,7 +890,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -906,7 +910,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -923,7 +927,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -940,7 +944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -957,7 +961,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -974,7 +978,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -989,7 +993,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1004,7 +1008,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1019,7 +1023,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1034,7 +1038,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1048,7 +1052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1076,7 +1080,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1090,7 +1094,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1104,7 +1108,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1118,7 +1122,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -1132,7 +1136,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1146,7 +1150,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
@@ -1160,7 +1164,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>3</v>
       </c>
@@ -1174,7 +1178,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1188,7 +1192,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -1225,19 +1229,19 @@
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -1260,7 +1264,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1277,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1294,10 +1298,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="C5" s="1"/>
     </row>
   </sheetData>
@@ -1317,21 +1321,21 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="140.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="140.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1339,7 +1343,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1347,7 +1351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1355,7 +1359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1374,25 +1378,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E63DFD8-2013-40A2-8CE5-0CB5ABE5CD54}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="140.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="140.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="63.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1417,8 +1422,11 @@
       <c r="H1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1435,7 +1443,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1449,7 +1457,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1463,7 +1471,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1474,7 +1482,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>60</v>
       </c>
@@ -1485,7 +1493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -1498,9 +1506,15 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="1">
+  <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{05490883-A9D0-4075-B059-A05DB8772F28}">
       <formula1>Modules</formula1>
+    </dataValidation>
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B159:B207" xr:uid="{6AF7A5D9-7551-45DF-9F21-74F221F8101D}">
+      <formula1>"ASSIGNMENT;URL;QUIZ;FILE;SUB_HEADER"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B158" xr:uid="{7641E481-7294-4CC9-8841-C4C7BFD46F1B}">
+      <formula1>"ASSIGNMENT,URL,QUIZ,FILE,SUB_HEADER"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1519,14 +1533,14 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>61</v>
       </c>
@@ -1537,7 +1551,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1548,7 +1562,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1559,7 +1573,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1570,7 +1584,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1581,7 +1595,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>

</xml_diff>